<commit_message>
Changed to use raw access to hardware
Also improved motion algorithm for stepper motors
ISR time min/max/avg = 0.43uS, 2.78uS, 1.39uS
</commit_message>
<xml_diff>
--- a/Tests/PipelinePlannerDesign/TrapezoidCalcs.xlsx
+++ b/Tests/PipelinePlannerDesign/TrapezoidCalcs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="37005" windowHeight="14505" xr2:uid="{C678E458-7B53-443E-8333-A8ABCC4677B1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23445" windowHeight="12420" xr2:uid="{C678E458-7B53-443E-8333-A8ABCC4677B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -240,13 +240,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.55</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.8</c:v>
+                  <c:v>87.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -258,16 +258,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1363,7 +1363,7 @@
   <dimension ref="B4:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1376,7 +1376,7 @@
         <v>6</v>
       </c>
       <c r="C4">
-        <v>10</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
@@ -1384,7 +1384,7 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
@@ -1392,7 +1392,7 @@
         <v>1</v>
       </c>
       <c r="C6">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
@@ -1400,7 +1400,7 @@
         <v>2</v>
       </c>
       <c r="C7">
-        <v>10</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
@@ -1408,7 +1408,7 @@
         <v>3</v>
       </c>
       <c r="C8">
-        <v>10</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
@@ -1417,7 +1417,7 @@
       </c>
       <c r="C10">
         <f xml:space="preserve"> (final*final-init*init) / 4 / acc + dist/2</f>
-        <v>5.1749999999999998</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
@@ -1426,7 +1426,7 @@
       </c>
       <c r="C11">
         <f xml:space="preserve"> C8-C10</f>
-        <v>4.8250000000000002</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
@@ -1435,7 +1435,7 @@
       </c>
       <c r="C15">
         <f>(feedrate*feedrate-init*init)/2/acc</f>
-        <v>4.55</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.25">
@@ -1453,7 +1453,7 @@
       </c>
       <c r="C17">
         <f>MIN($C$15,$C$10)</f>
-        <v>4.55</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
@@ -1462,7 +1462,7 @@
       </c>
       <c r="C18">
         <f>(feedrate*feedrate-final*final)/2/acc</f>
-        <v>4.2</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
@@ -1471,7 +1471,7 @@
       </c>
       <c r="C19">
         <f>IF($C$10&gt;$C$15,C18,C11)</f>
-        <v>4.2</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
@@ -1480,7 +1480,7 @@
       </c>
       <c r="C20">
         <f>C8-C17-C19</f>
-        <v>1.25</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
@@ -1500,7 +1500,7 @@
       </c>
       <c r="D25">
         <f>init</f>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
@@ -1509,11 +1509,11 @@
       </c>
       <c r="C26">
         <f>C17</f>
-        <v>4.55</v>
+        <v>12.5</v>
       </c>
       <c r="D26">
         <f>SQRT(init*init+2*C7*C17)</f>
-        <v>10</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
@@ -1522,11 +1522,11 @@
       </c>
       <c r="C27">
         <f>C20+C17</f>
-        <v>5.8</v>
+        <v>87.5</v>
       </c>
       <c r="D27">
         <f>D26</f>
-        <v>10</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
@@ -1535,11 +1535,11 @@
       </c>
       <c r="C28">
         <f>C8</f>
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="D28">
         <f>final</f>
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>